<commit_message>
arreglar envío de reglas a s3: se eliminó del flujo a RuleDate
</commit_message>
<xml_diff>
--- a/rules.xlsx
+++ b/rules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proyectos\Popular\Lambdas\sync_rules_lambda\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sblancof\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC110FE4-0A6C-412E-A3A3-8C5DDE87C97B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59EE5400-4AE6-4850-954E-B78F0349EBC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-4815" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{21AE682E-4C8F-4292-9C8F-B40B308DB341}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{21AE682E-4C8F-4292-9C8F-B40B308DB341}"/>
   </bookViews>
   <sheets>
     <sheet name="Presentación" sheetId="2" r:id="rId1"/>
@@ -32,87 +32,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>tc={AEFE7088-0E91-4234-97D3-BD13398C1896}</author>
-    <author>tc={C5EF2825-1FCA-4392-8B65-2C8F3CC47F4D}</author>
-    <author>tc={FFCB752E-44F2-422E-9E1A-EC23C436C750}</author>
-  </authors>
-  <commentList>
-    <comment ref="C13" authorId="0" shapeId="0" xr:uid="{5E6E4E66-1336-4EA6-BFCB-8C5854592A8C}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Según el estandar AVAL la estructura obligatoria para la respuesta:
-{
-  "MsgRsHdr": {
-    "Status": {
-      "StatusCode": "&lt;integer&gt;",
-      "Severity": "Info",
-      "StatusDesc": "&lt;string&gt;",
-      "AdditionalStatus": {
-        "StatusCode": "&lt;integer&gt;",
-        "StatusDesc": "&lt;string&gt;",
-        "ServerStatusCode": "&lt;integer&gt;",
-        "Severity": "Warning"
-      },
-      "ServerStatusCode": "&lt;integer&gt;",
-      "EndDt": "&lt;dateTime&gt;"
-    }
-  }
-}
-  </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C14" authorId="1" shapeId="0" xr:uid="{CA2416F1-9929-49C5-8EC6-E70DE178F6C0}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Los escenarios requeridos como insumo mínimo son:  Validación de estructura, estructuras correctas según condicionales del servicio.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C15" authorId="2" shapeId="0" xr:uid="{458342C1-CE42-4C2A-9DB6-AFD9D0DC94BB}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Los escenarios requeridos como insumo mínimo son:  Validación de estructura, estructuras correctas según condicionales del servicio.</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -383,13 +302,112 @@
     <cellStyle name="Incorrecto" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="21">
     <dxf>
       <font>
         <strike/>
         <color theme="0" tint="-0.499984740745262"/>
         <name val="Cambria"/>
         <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <name val="Cambria"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <name val="Cambria"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <name val="Cambria"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike/>
+        <color theme="0" tint="-0.499984740745262"/>
       </font>
     </dxf>
     <dxf>
@@ -471,9 +489,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -511,7 +529,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -617,7 +635,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -759,7 +777,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -773,188 +791,214 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDBF6345-24D7-4297-B079-BE485DF86473}">
-  <dimension ref="A2:F16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDBF6345-24D7-4297-B079-BE485DF86473}">
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="30.28515625" customWidth="1"/>
-    <col min="3" max="3" width="40.140625" customWidth="1"/>
-    <col min="4" max="4" width="29.7109375" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" customWidth="1"/>
-    <col min="6" max="6" width="35.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.26953125" customWidth="1"/>
+    <col min="3" max="3" width="40.1796875" customWidth="1"/>
+    <col min="4" max="4" width="29.7265625" customWidth="1"/>
+    <col min="5" max="5" width="21.7265625" customWidth="1"/>
+    <col min="6" max="6" width="35.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+    <row r="2" spans="1:6" ht="25" x14ac:dyDescent="0.35">
+      <c r="A2" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="E2" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="20" t="s">
+      <c r="F2" s="20" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="18"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="10"/>
       <c r="B5" s="11"/>
       <c r="C5" s="12"/>
       <c r="D5" s="13"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="5"/>
       <c r="B6" s="14"/>
       <c r="C6" s="15"/>
       <c r="D6" s="8"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="5"/>
       <c r="B7" s="6"/>
       <c r="C7" s="7"/>
       <c r="D7" s="8"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="5"/>
       <c r="B8" s="6"/>
       <c r="C8" s="7"/>
       <c r="D8" s="8"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="5"/>
       <c r="B9" s="16"/>
       <c r="C9" s="17"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="5"/>
       <c r="B10" s="6"/>
       <c r="C10" s="7"/>
       <c r="D10" s="8"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="5"/>
       <c r="B11" s="6"/>
       <c r="C11" s="7"/>
       <c r="D11" s="8"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
       <c r="C12" s="7"/>
       <c r="D12" s="8"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="18"/>
       <c r="B13" s="16"/>
       <c r="C13" s="17"/>
       <c r="D13" s="8"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="5"/>
       <c r="B14" s="16"/>
       <c r="C14" s="17"/>
       <c r="D14" s="8"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="5"/>
       <c r="B15" s="16"/>
       <c r="C15" s="17"/>
       <c r="D15" s="8"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="18"/>
       <c r="B16" s="16"/>
       <c r="C16" s="17"/>
       <c r="D16" s="8"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A3:C3 A5 A8 A10 A13 A16">
-    <cfRule type="expression" dxfId="8" priority="9" stopIfTrue="1">
-      <formula>$E3="R"</formula>
+  <conditionalFormatting sqref="A5 A8 A10 A13 A16">
+    <cfRule type="expression" dxfId="20" priority="14" stopIfTrue="1">
+      <formula>$E5="R"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:B16">
-    <cfRule type="expression" dxfId="7" priority="6">
+    <cfRule type="expression" dxfId="19" priority="11">
       <formula>$I4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:C16">
-    <cfRule type="expression" dxfId="6" priority="5">
+    <cfRule type="expression" dxfId="18" priority="10">
       <formula>$J4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C14">
+    <cfRule type="expression" dxfId="17" priority="13" stopIfTrue="1">
+      <formula>$E5="R"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B15:C16">
+    <cfRule type="expression" dxfId="16" priority="9" stopIfTrue="1">
+      <formula>$E15="R"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C4:C16">
+    <cfRule type="expression" dxfId="15" priority="12">
+      <formula>$I4=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D2 D4:D8">
     <cfRule type="expression" dxfId="5" priority="8" stopIfTrue="1">
-      <formula>$E5="R"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B15:C16">
-    <cfRule type="expression" dxfId="4" priority="4" stopIfTrue="1">
-      <formula>$E15="R"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C4:C16">
-    <cfRule type="expression" dxfId="3" priority="7">
-      <formula>$I4=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D8 D10:D14">
-    <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
-      <formula>$E3="R"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D15:D16">
-    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
-      <formula>$E15="R"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E3:F3">
+      <formula>$E1="R"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D10:D16">
+    <cfRule type="expression" dxfId="14" priority="7" stopIfTrue="1">
+      <formula>$E10="R"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:C1">
+    <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
+      <formula>$E1="R"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2">
+    <cfRule type="expression" dxfId="3" priority="3">
+      <formula>$I2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:C2">
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>$J2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2">
+    <cfRule type="expression" dxfId="1" priority="4">
+      <formula>$I2=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:F1">
     <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
-      <formula>$E3="R"</formula>
+      <formula>$E1="R"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>